<commit_message>
Excel-Datei 3 hat jetzt zweites Tabellenblatt
Damit soll getestet werden, dass nicht versehentlich ein falsches Tabellenblatt ausgelesen wird.
</commit_message>
<xml_diff>
--- a/src/main/resources/TestDateienFuerUnitTests/TestExcel_3_HappyPathFormel.xlsx
+++ b/src/main/resources/TestDateienFuerUnitTests/TestExcel_3_HappyPathFormel.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B831EFC5-F07F-4A97-B347-207CFAC7365B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA37E06-F710-43BF-91D5-22800B4970D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,12 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>xxx</t>
   </si>
   <si>
     <t>Test-Datei für den "Happy Path" (FORMULAR-Wert in Zelle A1 ist vorhanden)</t>
+  </si>
+  <si>
+    <t>Leeres Arbeitsblatt</t>
+  </si>
+  <si>
+    <t>Datei hat auch zweites Arbeitsblatt, das aber ignoriert werden sollte.</t>
   </si>
 </sst>
 </file>
@@ -72,10 +79,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -358,9 +368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -392,8 +404,39 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02741325-CEFB-4DF2-9BC1-3B6B35048EC9}">
+  <dimension ref="B3:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>